<commit_message>
Initial commit of Automation
</commit_message>
<xml_diff>
--- a/src/test/resource/TestData/Login.xlsx
+++ b/src/test/resource/TestData/Login.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="15">
   <si>
     <t xml:space="preserve">Username </t>
   </si>
@@ -59,6 +59,12 @@
   </si>
   <si>
     <t>Hi, John Smith</t>
+  </si>
+  <si>
+    <t>LOGIN</t>
+  </si>
+  <si>
+    <t>Hi, DVhbCERv IlqEZZxz</t>
   </si>
 </sst>
 </file>
@@ -492,7 +498,7 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E5" s="1"/>
     </row>

</xml_diff>